<commit_message>
Added multiThreading and Multiprocessing
</commit_message>
<xml_diff>
--- a/Result_data/DE_KNN_10_6.xlsx
+++ b/Result_data/DE_KNN_10_6.xlsx
@@ -4,15 +4,15 @@
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="18625"/>
   <workbookPr filterPrivacy="1"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView minimized="1" xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
-    <sheet name="Sheet3" sheetId="3" r:id="rId2"/>
-    <sheet name="Sheet2" sheetId="2" r:id="rId3"/>
+    <sheet name="Result" sheetId="1" r:id="rId1"/>
+    <sheet name="Class Avg" sheetId="5" r:id="rId2"/>
+    <sheet name="Calculation" sheetId="4" r:id="rId3"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$F$362</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Result!$A$1:$F$362</definedName>
   </definedNames>
   <calcPr calcId="171027"/>
   <extLst>
@@ -24,10 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="276" uniqueCount="8">
-  <si>
-    <t>Model training time:  4218.899186669406</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="283" uniqueCount="15">
   <si>
     <t>avg</t>
   </si>
@@ -48,6 +45,30 @@
   </si>
   <si>
     <t>Type</t>
+  </si>
+  <si>
+    <t>Precision Avg</t>
+  </si>
+  <si>
+    <t>Recall Avg</t>
+  </si>
+  <si>
+    <t>F-Score Avg</t>
+  </si>
+  <si>
+    <t>Class 1</t>
+  </si>
+  <si>
+    <t>Class 2</t>
+  </si>
+  <si>
+    <t>Class 3</t>
+  </si>
+  <si>
+    <t>Class 4</t>
+  </si>
+  <si>
+    <t>DE KNN</t>
   </si>
 </sst>
 </file>
@@ -368,8 +389,8 @@
   <sheetPr filterMode="1"/>
   <dimension ref="A1:F362"/>
   <sheetViews>
-    <sheetView topLeftCell="A72" workbookViewId="0">
-      <selection activeCell="E8" sqref="E8:E360"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I144" sqref="I144"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -379,19 +400,19 @@
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C1" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D1" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="E1" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F1" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="2" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
@@ -474,10 +495,10 @@
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B8" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C8">
         <v>0.83099999999999996</v>
@@ -497,16 +518,16 @@
         <v>9</v>
       </c>
       <c r="C9" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D9" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="E9" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F9" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="10" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
@@ -589,10 +610,10 @@
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B16" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C16">
         <v>0.92700000000000005</v>
@@ -612,16 +633,16 @@
         <v>9</v>
       </c>
       <c r="C17" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D17" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="E17" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F17" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="18" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
@@ -704,10 +725,10 @@
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B24" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C24">
         <v>0.93400000000000005</v>
@@ -727,16 +748,16 @@
         <v>9</v>
       </c>
       <c r="C25" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D25" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="E25" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F25" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="26" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
@@ -819,10 +840,10 @@
     </row>
     <row r="32" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B32" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C32">
         <v>0.92900000000000005</v>
@@ -842,16 +863,16 @@
         <v>9</v>
       </c>
       <c r="C33" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D33" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="E33" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F33" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="34" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
@@ -934,10 +955,10 @@
     </row>
     <row r="40" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B40" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C40">
         <v>0.93</v>
@@ -957,16 +978,16 @@
         <v>9</v>
       </c>
       <c r="C41" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D41" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="E41" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F41" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="42" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
@@ -1049,10 +1070,10 @@
     </row>
     <row r="48" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B48" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C48">
         <v>0.93100000000000005</v>
@@ -1072,16 +1093,16 @@
         <v>9</v>
       </c>
       <c r="C49" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D49" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="E49" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F49" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="50" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
@@ -1164,10 +1185,10 @@
     </row>
     <row r="56" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B56" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C56">
         <v>0.92800000000000005</v>
@@ -1187,16 +1208,16 @@
         <v>9</v>
       </c>
       <c r="C57" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D57" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="E57" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F57" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="58" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
@@ -1279,10 +1300,10 @@
     </row>
     <row r="64" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B64" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C64">
         <v>0.93300000000000005</v>
@@ -1302,16 +1323,16 @@
         <v>9</v>
       </c>
       <c r="C65" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D65" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="E65" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F65" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="66" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
@@ -1394,10 +1415,10 @@
     </row>
     <row r="72" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B72" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C72">
         <v>0.92500000000000004</v>
@@ -1417,16 +1438,16 @@
         <v>9</v>
       </c>
       <c r="C73" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D73" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="E73" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F73" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="74" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
@@ -1509,10 +1530,10 @@
     </row>
     <row r="80" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A80" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B80" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C80">
         <v>0.93200000000000005</v>
@@ -1532,16 +1553,16 @@
         <v>9</v>
       </c>
       <c r="C81" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D81" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="E81" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F81" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="82" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
@@ -1624,10 +1645,10 @@
     </row>
     <row r="88" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A88" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B88" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C88">
         <v>0.92900000000000005</v>
@@ -1647,16 +1668,16 @@
         <v>9</v>
       </c>
       <c r="C89" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D89" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="E89" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F89" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="90" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
@@ -1739,10 +1760,10 @@
     </row>
     <row r="96" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A96" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B96" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C96">
         <v>0.92900000000000005</v>
@@ -1762,16 +1783,16 @@
         <v>9</v>
       </c>
       <c r="C97" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D97" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="E97" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F97" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="98" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
@@ -1854,10 +1875,10 @@
     </row>
     <row r="104" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A104" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B104" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C104">
         <v>0.93300000000000005</v>
@@ -1877,16 +1898,16 @@
         <v>9</v>
       </c>
       <c r="C105" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D105" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="E105" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F105" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="106" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
@@ -1969,10 +1990,10 @@
     </row>
     <row r="112" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A112" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B112" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C112">
         <v>0.93600000000000005</v>
@@ -1992,16 +2013,16 @@
         <v>9</v>
       </c>
       <c r="C113" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D113" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="E113" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F113" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="114" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
@@ -2084,10 +2105,10 @@
     </row>
     <row r="120" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A120" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B120" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C120">
         <v>0.92700000000000005</v>
@@ -2107,16 +2128,16 @@
         <v>9</v>
       </c>
       <c r="C121" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D121" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="E121" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F121" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="122" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
@@ -2199,10 +2220,10 @@
     </row>
     <row r="128" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A128" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B128" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C128">
         <v>0.92800000000000005</v>
@@ -2222,16 +2243,16 @@
         <v>9</v>
       </c>
       <c r="C129" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D129" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="E129" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F129" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="130" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
@@ -2314,10 +2335,10 @@
     </row>
     <row r="136" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A136" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B136" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C136">
         <v>0.93400000000000005</v>
@@ -2337,16 +2358,16 @@
         <v>9</v>
       </c>
       <c r="C137" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D137" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="E137" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F137" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="138" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
@@ -2429,10 +2450,10 @@
     </row>
     <row r="144" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A144" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B144" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C144">
         <v>0.92900000000000005</v>
@@ -2452,16 +2473,16 @@
         <v>9</v>
       </c>
       <c r="C145" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D145" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="E145" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F145" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="146" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
@@ -2544,10 +2565,10 @@
     </row>
     <row r="152" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A152" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B152" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C152">
         <v>0.93799999999999994</v>
@@ -2567,16 +2588,16 @@
         <v>9</v>
       </c>
       <c r="C153" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D153" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="E153" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F153" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="154" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
@@ -2659,10 +2680,10 @@
     </row>
     <row r="160" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A160" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B160" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C160">
         <v>0.93200000000000005</v>
@@ -2682,16 +2703,16 @@
         <v>9</v>
       </c>
       <c r="C161" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D161" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="E161" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F161" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="162" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
@@ -2774,10 +2795,10 @@
     </row>
     <row r="168" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A168" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B168" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C168">
         <v>0.94199999999999995</v>
@@ -2797,16 +2818,16 @@
         <v>9</v>
       </c>
       <c r="C169" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D169" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="E169" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F169" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="170" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
@@ -2889,10 +2910,10 @@
     </row>
     <row r="176" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A176" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B176" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C176">
         <v>0.79600000000000004</v>
@@ -2912,16 +2933,16 @@
         <v>9</v>
       </c>
       <c r="C177" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D177" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="E177" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F177" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="178" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
@@ -3004,10 +3025,10 @@
     </row>
     <row r="184" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A184" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B184" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C184">
         <v>0.92700000000000005</v>
@@ -3027,16 +3048,16 @@
         <v>9</v>
       </c>
       <c r="C185" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D185" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="E185" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F185" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="186" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
@@ -3119,10 +3140,10 @@
     </row>
     <row r="192" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A192" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B192" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C192">
         <v>0.79600000000000004</v>
@@ -3142,16 +3163,16 @@
         <v>9</v>
       </c>
       <c r="C193" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D193" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="E193" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F193" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="194" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
@@ -3234,10 +3255,10 @@
     </row>
     <row r="200" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A200" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B200" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C200">
         <v>0.93200000000000005</v>
@@ -3257,16 +3278,16 @@
         <v>9</v>
       </c>
       <c r="C201" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D201" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="E201" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F201" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="202" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
@@ -3349,10 +3370,10 @@
     </row>
     <row r="208" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A208" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B208" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C208">
         <v>0.82599999999999996</v>
@@ -3372,16 +3393,16 @@
         <v>9</v>
       </c>
       <c r="C209" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D209" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="E209" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F209" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="210" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
@@ -3464,10 +3485,10 @@
     </row>
     <row r="216" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A216" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B216" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C216">
         <v>0.92500000000000004</v>
@@ -3487,16 +3508,16 @@
         <v>9</v>
       </c>
       <c r="C217" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D217" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="E217" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F217" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="218" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
@@ -3579,10 +3600,10 @@
     </row>
     <row r="224" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A224" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B224" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C224">
         <v>0.92500000000000004</v>
@@ -3602,16 +3623,16 @@
         <v>9</v>
       </c>
       <c r="C225" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D225" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="E225" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F225" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="226" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
@@ -3694,10 +3715,10 @@
     </row>
     <row r="232" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A232" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B232" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C232">
         <v>0.93</v>
@@ -3717,16 +3738,16 @@
         <v>9</v>
       </c>
       <c r="C233" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D233" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="E233" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F233" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="234" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
@@ -3809,10 +3830,10 @@
     </row>
     <row r="240" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A240" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B240" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C240">
         <v>0.84</v>
@@ -3832,16 +3853,16 @@
         <v>9</v>
       </c>
       <c r="C241" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D241" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="E241" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F241" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="242" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
@@ -3924,10 +3945,10 @@
     </row>
     <row r="248" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A248" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B248" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C248">
         <v>0.93600000000000005</v>
@@ -3947,16 +3968,16 @@
         <v>9</v>
       </c>
       <c r="C249" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D249" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="E249" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F249" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="250" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
@@ -4039,10 +4060,10 @@
     </row>
     <row r="256" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A256" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B256" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C256">
         <v>0.92700000000000005</v>
@@ -4062,16 +4083,16 @@
         <v>9</v>
       </c>
       <c r="C257" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D257" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="E257" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F257" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="258" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
@@ -4154,10 +4175,10 @@
     </row>
     <row r="264" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A264" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B264" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C264">
         <v>0.92600000000000005</v>
@@ -4177,16 +4198,16 @@
         <v>9</v>
       </c>
       <c r="C265" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D265" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="E265" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F265" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="266" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
@@ -4269,10 +4290,10 @@
     </row>
     <row r="272" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A272" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B272" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C272">
         <v>0.93799999999999994</v>
@@ -4292,16 +4313,16 @@
         <v>9</v>
       </c>
       <c r="C273" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D273" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="E273" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F273" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="274" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
@@ -4384,10 +4405,10 @@
     </row>
     <row r="280" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A280" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B280" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C280">
         <v>0.92800000000000005</v>
@@ -4407,16 +4428,16 @@
         <v>9</v>
       </c>
       <c r="C281" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D281" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="E281" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F281" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="282" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
@@ -4499,10 +4520,10 @@
     </row>
     <row r="288" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A288" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B288" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C288">
         <v>0.92600000000000005</v>
@@ -4522,16 +4543,16 @@
         <v>9</v>
       </c>
       <c r="C289" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D289" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="E289" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F289" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="290" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
@@ -4614,10 +4635,10 @@
     </row>
     <row r="296" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A296" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B296" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C296">
         <v>0.83399999999999996</v>
@@ -4637,16 +4658,16 @@
         <v>9</v>
       </c>
       <c r="C297" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D297" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="E297" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F297" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="298" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
@@ -4729,10 +4750,10 @@
     </row>
     <row r="304" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A304" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B304" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C304">
         <v>0.93200000000000005</v>
@@ -4752,16 +4773,16 @@
         <v>9</v>
       </c>
       <c r="C305" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D305" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="E305" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F305" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="306" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
@@ -4844,10 +4865,10 @@
     </row>
     <row r="312" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A312" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B312" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C312">
         <v>0.93200000000000005</v>
@@ -4867,16 +4888,16 @@
         <v>9</v>
       </c>
       <c r="C313" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D313" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="E313" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F313" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="314" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
@@ -4959,10 +4980,10 @@
     </row>
     <row r="320" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A320" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B320" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C320">
         <v>0.92600000000000005</v>
@@ -4982,16 +5003,16 @@
         <v>9</v>
       </c>
       <c r="C321" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D321" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="E321" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F321" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="322" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
@@ -5074,10 +5095,10 @@
     </row>
     <row r="328" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A328" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B328" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C328">
         <v>0.93100000000000005</v>
@@ -5097,16 +5118,16 @@
         <v>9</v>
       </c>
       <c r="C329" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D329" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="E329" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F329" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="330" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
@@ -5189,10 +5210,10 @@
     </row>
     <row r="336" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A336" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B336" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C336">
         <v>0.93</v>
@@ -5212,16 +5233,16 @@
         <v>9</v>
       </c>
       <c r="C337" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D337" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="E337" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F337" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="338" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
@@ -5304,10 +5325,10 @@
     </row>
     <row r="344" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A344" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B344" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C344">
         <v>0.92600000000000005</v>
@@ -5327,16 +5348,16 @@
         <v>9</v>
       </c>
       <c r="C345" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D345" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="E345" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F345" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="346" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
@@ -5419,10 +5440,10 @@
     </row>
     <row r="352" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A352" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B352" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C352">
         <v>0.93</v>
@@ -5442,16 +5463,16 @@
         <v>9</v>
       </c>
       <c r="C353" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D353" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="E353" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F353" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="354" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
@@ -5534,10 +5555,10 @@
     </row>
     <row r="360" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A360" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B360" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C360">
         <v>0.93500000000000005</v>
@@ -5557,16 +5578,16 @@
         <v>9</v>
       </c>
       <c r="C361" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D361" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="E361" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F361" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="362" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
@@ -5587,147 +5608,87 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{451938C5-E33E-494F-9327-E3C950F10434}">
-  <dimension ref="A1:AR1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F58776CC-B159-487F-BD19-8A9171F007C9}">
+  <dimension ref="A1:D5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:AR1"/>
+      <selection activeCell="C19" sqref="C19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="12.85546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="4" width="12" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:44" x14ac:dyDescent="0.25">
-      <c r="A1">
-        <v>0.82499999999999996</v>
-      </c>
-      <c r="B1">
-        <v>0.92500000000000004</v>
-      </c>
-      <c r="C1">
-        <v>0.93200000000000005</v>
-      </c>
-      <c r="D1">
-        <v>0.92700000000000005</v>
-      </c>
-      <c r="E1">
-        <v>0.92900000000000005</v>
-      </c>
-      <c r="F1">
-        <v>0.92800000000000005</v>
-      </c>
-      <c r="G1">
-        <v>0.92700000000000005</v>
-      </c>
-      <c r="H1">
-        <v>0.93200000000000005</v>
-      </c>
-      <c r="I1">
-        <v>0.92300000000000004</v>
-      </c>
-      <c r="J1">
-        <v>0.93</v>
-      </c>
-      <c r="K1">
-        <v>0.92700000000000005</v>
-      </c>
-      <c r="L1">
-        <v>0.92700000000000005</v>
-      </c>
-      <c r="M1">
-        <v>0.93200000000000005</v>
-      </c>
-      <c r="N1">
-        <v>0.93400000000000005</v>
-      </c>
-      <c r="O1">
-        <v>0.92600000000000005</v>
-      </c>
-      <c r="P1">
-        <v>0.92600000000000005</v>
-      </c>
-      <c r="Q1">
-        <v>0.93200000000000005</v>
-      </c>
-      <c r="R1">
-        <v>0.92700000000000005</v>
-      </c>
-      <c r="S1">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>14</v>
+      </c>
+      <c r="B1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>10</v>
+      </c>
+      <c r="B2">
+        <v>0.93847727272727299</v>
+      </c>
+      <c r="C2">
+        <v>0.86622727272727296</v>
+      </c>
+      <c r="D2">
+        <v>0.90068181818181792</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>11</v>
+      </c>
+      <c r="B3">
+        <v>0.85546666666666671</v>
+      </c>
+      <c r="C3">
+        <v>0.94000000000000006</v>
+      </c>
+      <c r="D3">
+        <v>0.89539999999999997</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>12</v>
+      </c>
+      <c r="B4">
         <v>0.93600000000000005</v>
       </c>
-      <c r="T1">
-        <v>0.93100000000000005</v>
-      </c>
-      <c r="U1">
-        <v>0.94099999999999995</v>
-      </c>
-      <c r="V1">
-        <v>0.78800000000000003</v>
-      </c>
-      <c r="W1">
-        <v>0.92600000000000005</v>
-      </c>
-      <c r="X1">
-        <v>0.78600000000000003</v>
-      </c>
-      <c r="Y1">
-        <v>0.93</v>
-      </c>
-      <c r="Z1">
-        <v>0.82099999999999995</v>
-      </c>
-      <c r="AA1">
-        <v>0.92400000000000004</v>
-      </c>
-      <c r="AB1">
-        <v>0.92200000000000004</v>
-      </c>
-      <c r="AC1">
-        <v>0.92700000000000005</v>
-      </c>
-      <c r="AD1">
-        <v>0.83499999999999996</v>
-      </c>
-      <c r="AE1">
-        <v>0.93400000000000005</v>
-      </c>
-      <c r="AF1">
-        <v>0.92600000000000005</v>
-      </c>
-      <c r="AG1">
-        <v>0.92400000000000004</v>
-      </c>
-      <c r="AH1">
-        <v>0.93700000000000006</v>
-      </c>
-      <c r="AI1">
-        <v>0.92600000000000005</v>
-      </c>
-      <c r="AJ1">
-        <v>0.92400000000000004</v>
-      </c>
-      <c r="AK1">
-        <v>0.82899999999999996</v>
-      </c>
-      <c r="AL1">
-        <v>0.93100000000000005</v>
-      </c>
-      <c r="AM1">
-        <v>0.93</v>
-      </c>
-      <c r="AN1">
-        <v>0.92300000000000004</v>
-      </c>
-      <c r="AO1">
-        <v>0.92800000000000005</v>
-      </c>
-      <c r="AP1">
-        <v>0.92800000000000005</v>
-      </c>
-      <c r="AQ1">
-        <v>0.92400000000000004</v>
-      </c>
-      <c r="AR1">
-        <v>0.92800000000000005</v>
+      <c r="C4">
+        <v>0.9932222222222219</v>
+      </c>
+      <c r="D4">
+        <v>0.96342222222222207</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>13</v>
+      </c>
+      <c r="B5">
+        <v>0.93320000000000003</v>
+      </c>
+      <c r="C5">
+        <v>0.85384444444444452</v>
+      </c>
+      <c r="D5">
+        <v>0.89086666666666681</v>
       </c>
     </row>
   </sheetData>
@@ -5736,158 +5697,522 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E22F51C0-CD80-4AC7-AC01-42E8035367E7}">
-  <dimension ref="A1:AT9"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0E158997-2CE1-49F8-8FF7-21D8920B8A37}">
+  <dimension ref="A1:C47"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A9" workbookViewId="0">
-      <selection activeCell="B9" sqref="B9:AT9"/>
+    <sheetView topLeftCell="A23" workbookViewId="0">
+      <selection activeCell="J24" sqref="J24:J68"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="37.42578125" bestFit="1" customWidth="1"/>
-  </cols>
   <sheetData>
-    <row r="1" spans="1:46" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="9" spans="1:46" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1">
+        <v>0.89</v>
+      </c>
+      <c r="B1">
+        <v>0.67</v>
+      </c>
+      <c r="C1">
+        <v>0.76500000000000001</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>0.93600000000000005</v>
+      </c>
+      <c r="B2">
+        <v>0.877</v>
+      </c>
+      <c r="C2">
+        <v>0.90600000000000003</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>0.94199999999999995</v>
+      </c>
+      <c r="B3">
+        <v>0.89</v>
+      </c>
+      <c r="C3">
+        <v>0.91500000000000004</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>0.94899999999999995</v>
+      </c>
+      <c r="B4">
+        <v>0.875</v>
+      </c>
+      <c r="C4">
+        <v>0.91</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>0.93200000000000005</v>
+      </c>
+      <c r="B5">
+        <v>0.88500000000000001</v>
+      </c>
+      <c r="C5">
+        <v>0.90800000000000003</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>0.95099999999999996</v>
+      </c>
+      <c r="B6">
+        <v>0.875</v>
+      </c>
+      <c r="C6">
+        <v>0.91100000000000003</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <v>0.94699999999999995</v>
+      </c>
+      <c r="B7">
+        <v>0.89</v>
+      </c>
+      <c r="C7">
+        <v>0.91800000000000004</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A8">
+        <v>0.95399999999999996</v>
+      </c>
+      <c r="B8">
+        <v>0.873</v>
+      </c>
+      <c r="C8">
+        <v>0.91100000000000003</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A9">
+        <v>0.94499999999999995</v>
+      </c>
       <c r="B9">
-        <v>0.82199999999999995</v>
+        <v>0.85299999999999998</v>
       </c>
       <c r="C9">
+        <v>0.89600000000000002</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A10">
+        <v>0.94599999999999995</v>
+      </c>
+      <c r="B10">
+        <v>0.88</v>
+      </c>
+      <c r="C10">
+        <v>0.91200000000000003</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A11">
+        <v>0.93899999999999995</v>
+      </c>
+      <c r="B11">
+        <v>0.88</v>
+      </c>
+      <c r="C11">
+        <v>0.90800000000000003</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A12">
+        <v>0.93600000000000005</v>
+      </c>
+      <c r="B12">
+        <v>0.88200000000000001</v>
+      </c>
+      <c r="C12">
+        <v>0.90900000000000003</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A13">
+        <v>0.94199999999999995</v>
+      </c>
+      <c r="B13">
+        <v>0.89</v>
+      </c>
+      <c r="C13">
+        <v>0.91500000000000004</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A14">
+        <v>0.94199999999999995</v>
+      </c>
+      <c r="B14">
+        <v>0.88700000000000001</v>
+      </c>
+      <c r="C14">
+        <v>0.91400000000000003</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A15">
+        <v>0.93400000000000005</v>
+      </c>
+      <c r="B15">
+        <v>0.877</v>
+      </c>
+      <c r="C15">
+        <v>0.90500000000000003</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A16">
+        <v>0.93400000000000005</v>
+      </c>
+      <c r="B16">
+        <v>0.89</v>
+      </c>
+      <c r="C16">
+        <v>0.91200000000000003</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A17">
+        <v>0.93899999999999995</v>
+      </c>
+      <c r="B17">
+        <v>0.89</v>
+      </c>
+      <c r="C17">
+        <v>0.91400000000000003</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A18">
+        <v>0.94399999999999995</v>
+      </c>
+      <c r="B18">
+        <v>0.88200000000000001</v>
+      </c>
+      <c r="C18">
+        <v>0.91200000000000003</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A19">
+        <v>0.94</v>
+      </c>
+      <c r="B19">
+        <v>0.90200000000000002</v>
+      </c>
+      <c r="C19">
+        <v>0.92100000000000004</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A20">
+        <v>0.93200000000000005</v>
+      </c>
+      <c r="B20">
+        <v>0.89500000000000002</v>
+      </c>
+      <c r="C20">
+        <v>0.91300000000000003</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A21">
+        <v>0.94799999999999995</v>
+      </c>
+      <c r="B21">
+        <v>0.91</v>
+      </c>
+      <c r="C21">
+        <v>0.92900000000000005</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A22">
+        <v>0.81899999999999995</v>
+      </c>
+      <c r="B22">
+        <v>0.65500000000000003</v>
+      </c>
+      <c r="C22">
+        <v>0.72799999999999998</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A23">
+        <v>0.93200000000000005</v>
+      </c>
+      <c r="B23">
+        <v>0.89</v>
+      </c>
+      <c r="C23">
+        <v>0.91</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A24">
+        <v>0.84699999999999998</v>
+      </c>
+      <c r="B24">
+        <v>0.63700000000000001</v>
+      </c>
+      <c r="C24">
+        <v>0.72799999999999998</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A25">
+        <v>0.95399999999999996</v>
+      </c>
+      <c r="B25">
+        <v>0.877</v>
+      </c>
+      <c r="C25">
+        <v>0.91400000000000003</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A26">
+        <v>0.874</v>
+      </c>
+      <c r="B26">
+        <v>0.67500000000000004</v>
+      </c>
+      <c r="C26">
+        <v>0.76200000000000001</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A27">
+        <v>0.93500000000000005</v>
+      </c>
+      <c r="B27">
+        <v>0.86499999999999999</v>
+      </c>
+      <c r="C27">
+        <v>0.89900000000000002</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A28">
+        <v>0.94599999999999995</v>
+      </c>
+      <c r="B28">
+        <v>0.875</v>
+      </c>
+      <c r="C28">
+        <v>0.90900000000000003</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A29">
+        <v>0.95599999999999996</v>
+      </c>
+      <c r="B29">
+        <v>0.86499999999999999</v>
+      </c>
+      <c r="C29">
+        <v>0.90800000000000003</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A30">
+        <v>0.89800000000000002</v>
+      </c>
+      <c r="B30">
+        <v>0.70299999999999996</v>
+      </c>
+      <c r="C30">
+        <v>0.78800000000000003</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A31">
+        <v>0.94199999999999995</v>
+      </c>
+      <c r="B31">
+        <v>0.89700000000000002</v>
+      </c>
+      <c r="C31">
+        <v>0.91900000000000004</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A32">
+        <v>0.94599999999999995</v>
+      </c>
+      <c r="B32">
+        <v>0.875</v>
+      </c>
+      <c r="C32">
+        <v>0.90900000000000003</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A33">
+        <v>0.93300000000000005</v>
+      </c>
+      <c r="B33">
+        <v>0.87</v>
+      </c>
+      <c r="C33">
+        <v>0.9</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A34">
+        <v>0.94399999999999995</v>
+      </c>
+      <c r="B34">
+        <v>0.89</v>
+      </c>
+      <c r="C34">
+        <v>0.91600000000000004</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A35">
+        <v>0.94899999999999995</v>
+      </c>
+      <c r="B35">
+        <v>0.875</v>
+      </c>
+      <c r="C35">
+        <v>0.91</v>
+      </c>
+    </row>
+    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A36">
+        <v>0.95</v>
+      </c>
+      <c r="B36">
+        <v>0.86299999999999999</v>
+      </c>
+      <c r="C36">
+        <v>0.90400000000000003</v>
+      </c>
+    </row>
+    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A37">
+        <v>0.89700000000000002</v>
+      </c>
+      <c r="B37">
+        <v>0.69799999999999995</v>
+      </c>
+      <c r="C37">
+        <v>0.78500000000000003</v>
+      </c>
+    </row>
+    <row r="38" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A38">
+        <v>0.94399999999999995</v>
+      </c>
+      <c r="B38">
+        <v>0.88</v>
+      </c>
+      <c r="C38">
+        <v>0.91100000000000003</v>
+      </c>
+    </row>
+    <row r="39" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A39">
+        <v>0.93700000000000006</v>
+      </c>
+      <c r="B39">
+        <v>0.89200000000000002</v>
+      </c>
+      <c r="C39">
+        <v>0.91400000000000003</v>
+      </c>
+    </row>
+    <row r="40" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A40">
+        <v>0.92300000000000004</v>
+      </c>
+      <c r="B40">
+        <v>0.9</v>
+      </c>
+      <c r="C40">
+        <v>0.91100000000000003</v>
+      </c>
+    </row>
+    <row r="41" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A41">
+        <v>0.96399999999999997</v>
+      </c>
+      <c r="B41">
+        <v>0.873</v>
+      </c>
+      <c r="C41">
+        <v>0.91600000000000004</v>
+      </c>
+    </row>
+    <row r="42" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A42">
+        <v>0.94399999999999995</v>
+      </c>
+      <c r="B42">
+        <v>0.88</v>
+      </c>
+      <c r="C42">
+        <v>0.91100000000000003</v>
+      </c>
+    </row>
+    <row r="43" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A43">
+        <v>0.93799999999999994</v>
+      </c>
+      <c r="B43">
+        <v>0.87</v>
+      </c>
+      <c r="C43">
+        <v>0.90300000000000002</v>
+      </c>
+    </row>
+    <row r="44" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A44">
+        <v>0.94299999999999995</v>
+      </c>
+      <c r="B44">
+        <v>0.87</v>
+      </c>
+      <c r="C44">
+        <v>0.90500000000000003</v>
+      </c>
+    </row>
+    <row r="45" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A45">
+        <v>0.95699999999999996</v>
+      </c>
+      <c r="B45">
+        <v>0.89500000000000002</v>
+      </c>
+      <c r="C45">
         <v>0.92500000000000004</v>
       </c>
-      <c r="D9">
-        <v>0.93200000000000005</v>
-      </c>
-      <c r="E9">
-        <v>0.92700000000000005</v>
-      </c>
-      <c r="F9">
-        <v>0.92800000000000005</v>
-      </c>
-      <c r="G9">
-        <v>0.92800000000000005</v>
-      </c>
-      <c r="H9">
-        <v>0.92700000000000005</v>
-      </c>
-      <c r="I9">
-        <v>0.93200000000000005</v>
-      </c>
-      <c r="J9">
-        <v>0.92300000000000004</v>
-      </c>
-      <c r="K9">
-        <v>0.93</v>
-      </c>
-      <c r="L9">
-        <v>0.92700000000000005</v>
-      </c>
-      <c r="M9">
-        <v>0.92700000000000005</v>
-      </c>
-      <c r="N9">
-        <v>0.93200000000000005</v>
-      </c>
-      <c r="O9">
-        <v>0.93400000000000005</v>
-      </c>
-      <c r="P9">
-        <v>0.92500000000000004</v>
-      </c>
-      <c r="Q9">
-        <v>0.92500000000000004</v>
-      </c>
-      <c r="R9">
-        <v>0.93200000000000005</v>
-      </c>
-      <c r="S9">
-        <v>0.92600000000000005</v>
-      </c>
-      <c r="T9">
-        <v>0.93500000000000005</v>
-      </c>
-      <c r="U9">
-        <v>0.93</v>
-      </c>
-      <c r="V9">
-        <v>0.94</v>
-      </c>
-      <c r="W9">
-        <v>0.78400000000000003</v>
-      </c>
-      <c r="X9">
-        <v>0.92500000000000004</v>
-      </c>
-      <c r="Y9">
-        <v>0.78200000000000003</v>
-      </c>
-      <c r="Z9">
-        <v>0.93</v>
-      </c>
-      <c r="AA9">
-        <v>0.81899999999999995</v>
-      </c>
-      <c r="AB9">
-        <v>0.92300000000000004</v>
-      </c>
-      <c r="AC9">
-        <v>0.92200000000000004</v>
-      </c>
-      <c r="AD9">
-        <v>0.92700000000000005</v>
-      </c>
-      <c r="AE9">
-        <v>0.83299999999999996</v>
-      </c>
-      <c r="AF9">
-        <v>0.93400000000000005</v>
-      </c>
-      <c r="AG9">
-        <v>0.92500000000000004</v>
-      </c>
-      <c r="AH9">
-        <v>0.92300000000000004</v>
-      </c>
-      <c r="AI9">
-        <v>0.93700000000000006</v>
-      </c>
-      <c r="AJ9">
-        <v>0.92600000000000005</v>
-      </c>
-      <c r="AK9">
-        <v>0.92300000000000004</v>
-      </c>
-      <c r="AL9">
-        <v>0.82699999999999996</v>
-      </c>
-      <c r="AM9">
-        <v>0.93</v>
-      </c>
-      <c r="AN9">
-        <v>0.93</v>
-      </c>
-      <c r="AO9">
-        <v>0.92300000000000004</v>
-      </c>
-      <c r="AP9">
-        <v>0.92800000000000005</v>
-      </c>
-      <c r="AQ9">
-        <v>0.92800000000000005</v>
-      </c>
-      <c r="AR9">
-        <v>0.92300000000000004</v>
-      </c>
-      <c r="AS9">
-        <v>0.92800000000000005</v>
-      </c>
-      <c r="AT9">
-        <v>0.93400000000000005</v>
+    </row>
+    <row r="47" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A47">
+        <f>AVERAGE(A1:A45)</f>
+        <v>0.93320000000000003</v>
+      </c>
+      <c r="B47">
+        <f t="shared" ref="B47:C47" si="0">AVERAGE(B1:B45)</f>
+        <v>0.85384444444444452</v>
+      </c>
+      <c r="C47">
+        <f t="shared" si="0"/>
+        <v>0.89086666666666681</v>
       </c>
     </row>
   </sheetData>

</xml_diff>